<commit_message>
Everythings works, except the interpolator keeps telling k not monotonic which happens with the HBW relations not with VGM.
</commit_message>
<xml_diff>
--- a/Stromingen/Munsflow_H2O_1995/data/NL_VG_soilprops.xlsx
+++ b/Stromingen/Munsflow_H2O_1995/data/NL_VG_soilprops.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/tools/Stromingen/Munsflow_H2O_1995/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027B818C-6E82-B04F-A8F6-18AC2D499C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57A48A4-2E1F-C943-8F68-68A5B3B97454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{F372BC66-B543-D943-98A8-6CF660848A41}"/>
   </bookViews>
@@ -745,18 +745,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CBB51C-C4C4-FB4A-8D08-99FB94CE3065}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.83203125" bestFit="1" customWidth="1"/>
@@ -771,28 +769,28 @@
         <v>110</v>
       </c>
       <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
         <v>105</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>108</v>
-      </c>
-      <c r="I1" t="s">
-        <v>109</v>
       </c>
       <c r="J1" t="s">
         <v>16</v>
@@ -816,25 +814,25 @@
     <row r="2" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
+      <c r="C2" s="3"/>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
       </c>
       <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="3"/>
       <c r="J2" t="s">
         <v>106</v>
       </c>
@@ -855,28 +853,28 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.02</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.42699999999999999</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2.1700000000000001E-2</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1.7350000000000001</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.98099999999999998</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>31.23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>52</v>
       </c>
       <c r="J3" t="s">
         <v>53</v>
@@ -899,28 +897,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.02</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.434</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1.349</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>7.202</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>83.24</v>
-      </c>
-      <c r="I4" t="s">
-        <v>56</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>94</v>
@@ -943,28 +941,28 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.02</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.443</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1.5049999999999999</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.13900000000000001</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>19.079999999999998</v>
-      </c>
-      <c r="I5" t="s">
-        <v>57</v>
       </c>
       <c r="J5" t="s">
         <v>58</v>
@@ -987,28 +985,28 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.02</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.46200000000000002</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1.49E-2</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>1.397</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.29499999999999998</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>34.880000000000003</v>
-      </c>
-      <c r="I6" t="s">
-        <v>59</v>
       </c>
       <c r="J6" t="s">
         <v>60</v>
@@ -1031,28 +1029,28 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.01</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.38100000000000001</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1.8080000000000001</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>2.4E-2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>63.65</v>
-      </c>
-      <c r="I7" t="s">
-        <v>61</v>
       </c>
       <c r="L7" t="s">
         <v>54</v>
@@ -1072,28 +1070,28 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.01</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.38500000000000001</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>1.242</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>-1.2</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>104.1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>63</v>
       </c>
       <c r="J8" t="s">
         <v>64</v>
@@ -1116,28 +1114,28 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.40100000000000002</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>1.83E-2</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>1.248</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.95199999999999996</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>14.58</v>
-      </c>
-      <c r="I9" t="s">
-        <v>66</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>95</v>
@@ -1157,28 +1155,28 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.01</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.433</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1.278</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>-1.919</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>3</v>
-      </c>
-      <c r="I10" t="s">
-        <v>67</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>96</v>
@@ -1198,28 +1196,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
         <v>68</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.43</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>1.2669999999999999</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>-2.387</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>1.75</v>
-      </c>
-      <c r="I11" t="s">
-        <v>69</v>
       </c>
       <c r="K11" t="s">
         <v>70</v>
@@ -1239,28 +1237,28 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.01</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.44800000000000001</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1.135</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>4.5810000000000004</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>3.83</v>
-      </c>
-      <c r="I12" t="s">
-        <v>71</v>
       </c>
       <c r="K12" t="s">
         <v>72</v>
@@ -1280,28 +1278,28 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.01</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>0.59099999999999997</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>1.107</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>-5.5490000000000004</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>6.31</v>
-      </c>
-      <c r="I13" t="s">
-        <v>73</v>
       </c>
       <c r="K13" t="s">
         <v>74</v>
@@ -1321,28 +1319,28 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.01</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>0.53</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>1.66E-2</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>1.091</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>-4.4939999999999998</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>2.25</v>
-      </c>
-      <c r="I14" t="s">
-        <v>75</v>
       </c>
       <c r="K14" t="s">
         <v>76</v>
@@ -1362,28 +1360,28 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.01</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>0.41599999999999998</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>1.4370000000000001</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>-1.357</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>29.83</v>
-      </c>
-      <c r="I15" t="s">
-        <v>77</v>
       </c>
       <c r="J15" t="s">
         <v>78</v>
@@ -1403,28 +1401,28 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
         <v>18</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.01</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>0.41699999999999998</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>5.4000000000000003E-3</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>1.302</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>-0.33500000000000002</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>0.9</v>
-      </c>
-      <c r="I16" t="s">
-        <v>79</v>
       </c>
       <c r="J16" t="s">
         <v>80</v>
@@ -1444,28 +1442,28 @@
         <v>81</v>
       </c>
       <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
         <v>19</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>0.01</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>0.52800000000000002</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>2.3699999999999999E-2</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>1.282</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>-1.478</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>87.45</v>
-      </c>
-      <c r="I17" t="s">
-        <v>82</v>
       </c>
       <c r="K17" t="s">
         <v>83</v>
@@ -1485,28 +1483,28 @@
         <v>81</v>
       </c>
       <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
         <v>20</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>0.01</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>0.78600000000000003</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>2.1100000000000001E-2</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>1.2789999999999999</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>-1.2210000000000001</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>12.36</v>
-      </c>
-      <c r="I18" t="s">
-        <v>85</v>
       </c>
       <c r="K18" t="s">
         <v>83</v>
@@ -1526,28 +1524,28 @@
         <v>81</v>
       </c>
       <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" t="s">
         <v>21</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>0</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>0.71899999999999997</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>1.9099999999999999E-2</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>1.137</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>0</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>4.4800000000000004</v>
-      </c>
-      <c r="I19" t="s">
-        <v>87</v>
       </c>
       <c r="K19" t="s">
         <v>88</v>
@@ -1567,28 +1565,28 @@
         <v>81</v>
       </c>
       <c r="B20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>0</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>0.76500000000000001</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>2.0500000000000001E-2</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>1.151</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>0</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>13.14</v>
-      </c>
-      <c r="I20" t="s">
-        <v>90</v>
       </c>
       <c r="K20" t="s">
         <v>88</v>
@@ -1608,28 +1606,28 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
         <v>31</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>0.01</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>0.36599999999999999</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>1.6E-2</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>2.1629999999999998</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>2.8679999999999999</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>22.32</v>
-      </c>
-      <c r="I21" t="s">
-        <v>52</v>
       </c>
       <c r="J21" t="s">
         <v>53</v>
@@ -1652,28 +1650,28 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
         <v>32</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>0.02</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>0.38700000000000001</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>1.61E-2</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>1.524</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>2.44</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>22.76</v>
-      </c>
-      <c r="I22" t="s">
-        <v>56</v>
       </c>
       <c r="J22" s="1">
         <v>45948</v>
@@ -1696,28 +1694,28 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
         <v>33</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>0.01</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>0.34</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>1.72E-2</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>1.7030000000000001</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>0</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>12.37</v>
-      </c>
-      <c r="I23" t="s">
-        <v>57</v>
       </c>
       <c r="J23" t="s">
         <v>58</v>
@@ -1740,28 +1738,28 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
         <v>34</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>0.01</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>0.36399999999999999</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>1.488</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>2.1789999999999998</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>25.81</v>
-      </c>
-      <c r="I24" t="s">
-        <v>59</v>
       </c>
       <c r="J24" t="s">
         <v>60</v>
@@ -1784,28 +1782,28 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
         <v>35</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>0.01</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>0.33700000000000002</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>3.0300000000000001E-2</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>2.8879999999999999</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>17.420000000000002</v>
-      </c>
-      <c r="I25" t="s">
-        <v>61</v>
       </c>
       <c r="L25" t="s">
         <v>97</v>
@@ -1825,28 +1823,28 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" t="s">
         <v>36</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>0.01</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>0.33300000000000002</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>1.6E-2</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>1.2889999999999999</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>-1.01</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>32.83</v>
-      </c>
-      <c r="I26" t="s">
-        <v>63</v>
       </c>
       <c r="J26" t="s">
         <v>64</v>
@@ -1869,28 +1867,28 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" t="s">
         <v>37</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>0.01</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>0.51300000000000001</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>1.2E-2</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>1.153</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>-2.0129999999999999</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>37.549999999999997</v>
-      </c>
-      <c r="I27" t="s">
-        <v>98</v>
       </c>
       <c r="J27" t="s">
         <v>60</v>
@@ -1913,28 +1911,28 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
         <v>38</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>0</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>0.45400000000000001</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>1.1299999999999999E-2</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>1.3460000000000001</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>-0.90400000000000003</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>8.64</v>
-      </c>
-      <c r="I28" t="s">
-        <v>66</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>95</v>
@@ -1954,28 +1952,28 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
         <v>39</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>0</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>0.45800000000000002</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>1.3759999999999999</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>-1.0129999999999999</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>3.77</v>
-      </c>
-      <c r="I29" t="s">
-        <v>67</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>96</v>
@@ -1995,28 +1993,28 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
         <v>40</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>0.01</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>0.47199999999999998</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>0.01</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>1.246</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>-0.79300000000000004</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>2.2999999999999998</v>
-      </c>
-      <c r="I30" t="s">
-        <v>69</v>
       </c>
       <c r="K30" t="s">
         <v>70</v>
@@ -2036,28 +2034,28 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
         <v>41</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>0</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>0.44400000000000001</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>1.43E-2</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>1.1259999999999999</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>2.3570000000000002</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>2.12</v>
-      </c>
-      <c r="I31" t="s">
-        <v>71</v>
       </c>
       <c r="K31" t="s">
         <v>72</v>
@@ -2077,28 +2075,28 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" t="s">
         <v>42</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>0.01</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>0.56100000000000005</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>1.1579999999999999</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>-3.1720000000000002</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>1.08</v>
-      </c>
-      <c r="I32" t="s">
-        <v>73</v>
       </c>
       <c r="K32" t="s">
         <v>74</v>
@@ -2118,28 +2116,28 @@
         <v>23</v>
       </c>
       <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s">
         <v>43</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>0.01</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>0.57299999999999995</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>2.7900000000000001E-2</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>1.08</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>-6.0910000000000002</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>9.69</v>
-      </c>
-      <c r="I33" t="s">
-        <v>75</v>
       </c>
       <c r="K33" t="s">
         <v>76</v>
@@ -2159,28 +2157,28 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
         <v>44</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>0.01</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>0.39400000000000002</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>3.3E-3</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>1.617</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>0.51400000000000001</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>2.5</v>
-      </c>
-      <c r="I34" t="s">
-        <v>77</v>
       </c>
       <c r="J34" t="s">
         <v>78</v>
@@ -2200,28 +2198,28 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" t="s">
         <v>45</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>0.01</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>0.41</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>7.7999999999999996E-3</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>1.2869999999999999</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>0</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>2.79</v>
-      </c>
-      <c r="I35" t="s">
-        <v>79</v>
       </c>
       <c r="J35" t="s">
         <v>80</v>
@@ -2241,28 +2239,28 @@
         <v>24</v>
       </c>
       <c r="B36" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" t="s">
         <v>46</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>0</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>0.88900000000000001</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>1.3640000000000001</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>-0.66500000000000004</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>1.46</v>
-      </c>
-      <c r="I36" t="s">
-        <v>100</v>
       </c>
       <c r="L36" t="s">
         <v>101</v>
@@ -2279,28 +2277,28 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
         <v>47</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>0.01</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>0.84899999999999998</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>1.1900000000000001E-2</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>1.272</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>-1.2490000000000001</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>3.4</v>
-      </c>
-      <c r="I37" t="s">
-        <v>102</v>
       </c>
       <c r="L37" t="s">
         <v>101</v>
@@ -2317,28 +2315,28 @@
         <v>24</v>
       </c>
       <c r="B38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" t="s">
         <v>48</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>0.01</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>1.3160000000000001</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>-0.78600000000000003</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>35.950000000000003</v>
-      </c>
-      <c r="I38" t="s">
-        <v>103</v>
       </c>
       <c r="L38" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
Checked again. It's about ok.
</commit_message>
<xml_diff>
--- a/Stromingen/Munsflow_H2O_1995/data/NL_VG_soilprops.xlsx
+++ b/Stromingen/Munsflow_H2O_1995/data/NL_VG_soilprops.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/tools/Stromingen/Munsflow_H2O_1995/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EBEC56-DF8B-7948-8BE1-D6BEB1888A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81810CD4-D0E2-5449-BCDD-B02F2847651F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="2360" windowWidth="34980" windowHeight="19240" activeTab="2" xr2:uid="{F372BC66-B543-D943-98A8-6CF660848A41}"/>
+    <workbookView xWindow="760" yWindow="2340" windowWidth="34980" windowHeight="19240" activeTab="2" xr2:uid="{F372BC66-B543-D943-98A8-6CF660848A41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>